<commit_message>
* refine custom function example - leave just one tld to avoid confusion - update taglib URI - update example xlsx file
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/customFunction.xlsx
+++ b/src/main/webapp/WEB-INF/books/customFunction.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80525671-0A32-3E49-8E32-C5382A503B79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="21075" windowHeight="9270" activeTab="1"/>
+    <workbookView xWindow="3020" yWindow="860" windowWidth="21040" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="custom-formula" sheetId="1" r:id="rId1"/>
+    <sheet name="custom function" sheetId="1" r:id="rId1"/>
     <sheet name="CHAIN" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>MYSUBTOTAL</t>
   </si>
@@ -99,13 +105,22 @@
   </si>
   <si>
     <t xml:space="preserve"> =CHAIN(D8,E8,F8,G8)</t>
+  </si>
+  <si>
+    <t>Custom Function</t>
+  </si>
+  <si>
+    <t>Custom function</t>
+  </si>
+  <si>
+    <t>Function Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +165,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -210,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -219,17 +242,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -276,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,9 +342,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,6 +394,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,186 +587,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="7" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="7" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
-      <c r="A1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="e">
+        <f ca="1">EXCHANGE(D4,E4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="e">
-        <f ca="1">EXCHANGE(D3,E3)</f>
+      <c r="E4">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="e">
+        <f ca="1">MYEXCHANGE(D6, E6)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>31.3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="e">
-        <f ca="1">MYEXCHANGE(D5, E5)</f>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="e">
+        <f ca="1">MYSUBTOTAL(D8:G8)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>31.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75">
-      <c r="A7" s="1" t="s">
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="e">
+        <f ca="1">MYSUBTOTAL(D10:G10)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="e">
+        <f ca="1">MYSUBTOTAL(D12:G12)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D12">
+        <v>1.5</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="e">
-        <f ca="1">MYSUBTOTAL(D7:G7)</f>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="e">
+        <f ca="1">MYSUBTOTAL(D14, E14, F14, G14)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D7">
+      <c r="D14">
         <v>1.5</v>
       </c>
-      <c r="E7">
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="G7">
+      <c r="G14">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="e">
-        <f ca="1">MYSUBTOTAL(D9:G9)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D9">
-        <v>1.5</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2" t="e">
-        <f ca="1">MYSUBTOTAL(D11:G11)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D11">
-        <v>1.5</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2" t="e">
-        <f ca="1">MYSUBTOTAL(D13, E13, F13, G13)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D13">
-        <v>1.5</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:G1"/>
+  <mergeCells count="2">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -704,21 +782,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -728,14 +806,14 @@
       <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -751,7 +829,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -760,7 +838,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -784,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -793,7 +871,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -815,7 +893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -824,7 +902,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>